<commit_message>
discussion - minor issues fixed
</commit_message>
<xml_diff>
--- a/data/input/SimulatorScenarios.xlsx
+++ b/data/input/SimulatorScenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonWorkspace\ABMSimulationTool\ABMSim\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemju/Desktop/AI_ML/ABMSim/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC40DDFB-4746-4EAB-822D-00C514A3C407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DDEC6F-950B-0C40-80C8-BD9353BC3279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7700" yWindow="0" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -122,15 +122,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,20 +406,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.08984375" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.453125" customWidth="1"/>
-    <col min="9" max="9" width="23.453125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -449,7 +446,7 @@
       <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -467,10 +464,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
         <v>10</v>
-      </c>
-      <c r="D2" s="1">
-        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -484,7 +481,7 @@
       <c r="H2" s="2">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1">
@@ -502,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
         <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -519,7 +516,7 @@
       <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="1">
@@ -537,10 +534,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
         <v>10</v>
-      </c>
-      <c r="D4" s="1">
-        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
@@ -554,7 +551,7 @@
       <c r="H4" s="2">
         <v>1</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="1">
@@ -572,10 +569,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
         <v>10</v>
-      </c>
-      <c r="D5" s="1">
-        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>6</v>
@@ -589,7 +586,7 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J5" s="1">

</xml_diff>

<commit_message>
minor fixes on Visualisations
</commit_message>
<xml_diff>
--- a/data/input/SimulatorScenarios.xlsx
+++ b/data/input/SimulatorScenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemju/Desktop/AI_ML/ABMSim/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DDEC6F-950B-0C40-80C8-BD9353BC3279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A7FCF4-C5A3-0643-AD97-DA3753FADA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="0" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="1040" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -467,7 +467,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -537,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
@@ -572,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>6</v>

</xml_diff>